<commit_message>
Updated with new data
</commit_message>
<xml_diff>
--- a/Body.xlsx
+++ b/Body.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ecommerce_Manual_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D436941C-F296-4358-BE5E-E68DA87B9C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5975302D-58A3-44F2-ABC0-83F2A91E953A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8B6476ED-93B3-458B-9892-B3A890F15F56}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="110">
   <si>
     <t>Product name</t>
   </si>
@@ -328,6 +328,42 @@
   </si>
   <si>
     <t>There shouldn't be any useless texts on body which are irrelavent</t>
+  </si>
+  <si>
+    <t>Images should be displayed properly</t>
+  </si>
+  <si>
+    <t>Alt texts should be added for the specific images</t>
+  </si>
+  <si>
+    <t>Images should be resizied in different screen sizes</t>
+  </si>
+  <si>
+    <t>All images shouldn't be in same sizes</t>
+  </si>
+  <si>
+    <t>There should be perfect alignment of the pictures for the particular sections</t>
+  </si>
+  <si>
+    <t>Resolutions of the pictures should be high and responsive</t>
+  </si>
+  <si>
+    <t>Image color shouldn't be same for the sections on which it's been placed</t>
+  </si>
+  <si>
+    <t>Images shouldn't be overlapping</t>
+  </si>
+  <si>
+    <t>Buttons shoudn't be create any problem on displaying on images</t>
+  </si>
+  <si>
+    <t>Text and text color on images should be responsive</t>
+  </si>
+  <si>
+    <t>alt text of the images shouldn't be broken</t>
+  </si>
+  <si>
+    <t>Images should be specified and related to the sections</t>
   </si>
 </sst>
 </file>
@@ -979,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA19025C-277F-4DBB-BB44-9F0A648F386E}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1647,9 @@
       <c r="E39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1641,7 +1679,9 @@
       <c r="E41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -1671,7 +1711,9 @@
       <c r="E43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1701,7 +1743,9 @@
       <c r="E45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -1731,7 +1775,9 @@
       <c r="E47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1761,7 +1807,9 @@
       <c r="E49" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -1791,7 +1839,9 @@
       <c r="E51" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -1821,7 +1871,9 @@
       <c r="E53" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -1851,7 +1903,9 @@
       <c r="E55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -1881,7 +1935,9 @@
       <c r="E57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -1911,7 +1967,9 @@
       <c r="E59" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
@@ -1941,7 +1999,9 @@
       <c r="E61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>

</xml_diff>